<commit_message>
add print time for the evaluation test
</commit_message>
<xml_diff>
--- a/test/regression/YearPredictMSD, normalized/loss_log_analysis-2016-03-28.xlsx
+++ b/test/regression/YearPredictMSD, normalized/loss_log_analysis-2016-03-28.xlsx
@@ -9,12 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15940" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15940" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="regression, logistic, accelerat" sheetId="3" r:id="rId1"/>
     <sheet name="size of inner loop" sheetId="4" r:id="rId2"/>
     <sheet name="Sheet2" sheetId="5" r:id="rId3"/>
+    <sheet name="no trick, DisSVRG" sheetId="6" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="loss_10" localSheetId="0">'regression, logistic, accelerat'!#REF!</definedName>
@@ -209,7 +210,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
   <si>
     <t>logistic regression</t>
   </si>
@@ -257,6 +258,12 @@
   </si>
   <si>
     <t xml:space="preserve">loss </t>
+  </si>
+  <si>
+    <t>without trick,</t>
+  </si>
+  <si>
+    <t>5-machines</t>
   </si>
 </sst>
 </file>
@@ -13056,8 +13063,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M1835"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1:I700"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -37177,4 +37184,39 @@
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>